<commit_message>
satan's on a rampage!
</commit_message>
<xml_diff>
--- a/Utilities/collisionMapping.xlsx
+++ b/Utilities/collisionMapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="11">
   <si>
     <t>Player</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>Satan</t>
+  </si>
+  <si>
+    <t>Gore</t>
   </si>
 </sst>
 </file>
@@ -660,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,15 +826,15 @@
       <c r="J6" s="12">
         <v>1</v>
       </c>
-      <c r="K6" s="13">
-        <v>0</v>
-      </c>
-      <c r="L6" s="14">
-        <v>0</v>
+      <c r="K6" s="12">
+        <v>1</v>
+      </c>
+      <c r="L6" s="12">
+        <v>1</v>
       </c>
       <c r="M6" s="5">
         <f>SUMPRODUCT($E$4:$L$4, $E6:$L6)</f>
-        <v>60</v>
+        <v>252</v>
       </c>
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
@@ -921,12 +924,12 @@
       <c r="K9" s="13">
         <v>0</v>
       </c>
-      <c r="L9" s="14">
-        <v>0</v>
+      <c r="L9" s="12">
+        <v>1</v>
       </c>
       <c r="M9" s="5">
         <f>SUMPRODUCT($E$4:$L$4, $E9:$L9)</f>
-        <v>4</v>
+        <v>132</v>
       </c>
       <c r="N9" s="19"/>
       <c r="O9" s="19"/>
@@ -1001,8 +1004,8 @@
       <c r="F12" s="12">
         <v>1</v>
       </c>
-      <c r="G12" s="12">
-        <v>1</v>
+      <c r="G12" s="13">
+        <v>0</v>
       </c>
       <c r="H12" s="13">
         <v>0</v>
@@ -1013,15 +1016,15 @@
       <c r="J12" s="13">
         <v>0</v>
       </c>
-      <c r="K12" s="13">
-        <v>0</v>
+      <c r="K12" s="12">
+        <v>1</v>
       </c>
       <c r="L12" s="14">
         <v>0</v>
       </c>
       <c r="M12" s="5">
         <f>SUMPRODUCT($E$4:$L$4, $E12:$L12)</f>
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
@@ -1198,18 +1201,18 @@
       <c r="I18" s="13">
         <v>0</v>
       </c>
-      <c r="J18" s="12">
-        <v>1</v>
+      <c r="J18" s="13">
+        <v>0</v>
       </c>
       <c r="K18" s="13">
         <v>0</v>
       </c>
-      <c r="L18" s="14">
-        <v>0</v>
+      <c r="L18" s="12">
+        <v>1</v>
       </c>
       <c r="M18" s="5">
         <f>SUMPRODUCT($E$4:$L$4, $E18:$L18)</f>
-        <v>37</v>
+        <v>133</v>
       </c>
       <c r="N18" s="19"/>
       <c r="O18" s="19"/>
@@ -1284,8 +1287,8 @@
       <c r="H21" s="13">
         <v>0</v>
       </c>
-      <c r="I21" s="12">
-        <v>1</v>
+      <c r="I21" s="13">
+        <v>0</v>
       </c>
       <c r="J21" s="13">
         <v>0</v>
@@ -1298,7 +1301,7 @@
       </c>
       <c r="M21" s="5">
         <f>SUMPRODUCT($E$4:$L$4, $E21:$L21)</f>
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1376,12 +1379,95 @@
       <c r="K24" s="13">
         <v>0</v>
       </c>
-      <c r="L24" s="14">
-        <v>0</v>
+      <c r="L24" s="12">
+        <v>1</v>
       </c>
       <c r="M24" s="5">
         <f>SUMPRODUCT($E$4:$L$4, $E24:$L24)</f>
-        <v>5</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="18"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="6"/>
+    </row>
+    <row r="26" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>0</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0</v>
+      </c>
+      <c r="I26" s="9">
+        <v>0</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0</v>
+      </c>
+      <c r="L26" s="8">
+        <v>1</v>
+      </c>
+      <c r="M26" s="5">
+        <f>SUMPRODUCT($E$4:$L$4, $E26:$L26)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="21"/>
+      <c r="D27" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" s="12">
+        <v>1</v>
+      </c>
+      <c r="F27" s="12">
+        <v>1</v>
+      </c>
+      <c r="G27" s="13">
+        <v>0</v>
+      </c>
+      <c r="H27" s="13">
+        <v>0</v>
+      </c>
+      <c r="I27" s="12">
+        <v>1</v>
+      </c>
+      <c r="J27" s="13">
+        <v>0</v>
+      </c>
+      <c r="K27" s="12">
+        <v>1</v>
+      </c>
+      <c r="L27" s="12">
+        <v>1</v>
+      </c>
+      <c r="M27" s="5">
+        <f>SUMPRODUCT($E$4:$L$4, $E27:$L27)</f>
+        <v>211</v>
       </c>
     </row>
   </sheetData>

</xml_diff>